<commit_message>
Alterações realizadas a pedido do GT Dados
Incluídos, na estrutura dos cartões, serviços prioritários e outros serviços, dentro da estrutura de 'fees'.
Para PJ, foi incluído o bloco 'services' dentro de fees.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
+++ b/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23107"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEA8E111-3C4B-4134-85E8-9EEE61A48E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7170" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7170" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContaPgtoPagoPF" sheetId="4" r:id="rId1"/>
     <sheet name="ContaPgtoPagoPJ " sheetId="6" r:id="rId2"/>
     <sheet name="Naturezas" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,11 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="80">
   <si>
     <t>Xpath</t>
   </si>
   <si>
+    <t>Nome</t>
+  </si>
+  <si>
     <t>Definição</t>
   </si>
   <si>
@@ -66,6 +70,12 @@
     <t>Restrições</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Nome do conglomerado proprietário da companhia responsável pelas contas de pagamento pós-pagas (cartão de crédito)</t>
+  </si>
+  <si>
     <t>Texto</t>
   </si>
   <si>
@@ -78,163 +88,30 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Naturezas válidas: 
-Código, 
-Data, 
-Descrição, 
-Hora, 
-Indicador (Flag), 
-Nome, 
-Número, 
-Percentual, 
-Quantidade, 
-Texto, 
-Valor</t>
-  </si>
-  <si>
-    <t>Opcional</t>
-  </si>
-  <si>
-    <t>1 saque a crédito
-2 outros</t>
-  </si>
-  <si>
-    <t>Nome do conglomerado proprietário da companhia responsável pelas contas de pagamento pós-pagas (cartão de crédito)</t>
-  </si>
-  <si>
-    <t>Booleano</t>
-  </si>
-  <si>
-    <t>1 VISA 
-2 MasterCard 
-3 American Express 
-4 Diners Club 
-5 Hipercard 
-6 Bandeira própria 
-7 Cheque Eletrônico 
-8 Elo 
-99 Outras</t>
-  </si>
-  <si>
-    <t>^([A-Z]{3})$</t>
-  </si>
-  <si>
-    <t>1 Classic Nacional
-2 Classic Internacional
-3 Gold
-4 Platinum
-5 Infinite
-6 Electron
-7 Standard Nacional
-8 Standard Internacional</t>
-  </si>
-  <si>
-    <t>Enum</t>
-  </si>
-  <si>
-    <t>brandCode</t>
-  </si>
-  <si>
-    <t>productType</t>
-  </si>
-  <si>
-    <t>name</t>
+    <t>Nome da Instituição, pertencente à organização, responsável pelas contas de pagamento pós-pagas (cartões de crédito) Ex. 'Empresa da Organização A'</t>
   </si>
   <si>
     <t>cnpjNumber</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>isPrivateLabel</t>
-  </si>
-  <si>
-    <t>priorityServiceName</t>
-  </si>
-  <si>
-    <t>maxPrice</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>elegibilityCriteriaInfo</t>
-  </si>
-  <si>
-    <t>closingProcessInfo</t>
-  </si>
-  <si>
-    <t>feeRate</t>
-  </si>
-  <si>
-    <t>instalmentRate</t>
-  </si>
-  <si>
-    <t>minimumFeeRate</t>
-  </si>
-  <si>
-    <t>Campo aberto para detalhamento de taxas de juros.</t>
-  </si>
-  <si>
-    <t>^(\d{14})$</t>
-  </si>
-  <si>
-    <t>^([0-1]{1})$</t>
   </si>
   <si>
     <t>Número completo do CNPJ da instituição responsável pelas contas de pagamento pós-pagas (cartões de crédito) - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'  Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
 Deve-se ter apenas os números do CNPJ, sem máscara.</t>
   </si>
   <si>
+    <t>^(\d{14})$</t>
+  </si>
+  <si>
     <t>Números de 0 a 9.</t>
-  </si>
-  <si>
-    <t>(\d{1,9}\,\d{2}){1}</t>
-  </si>
-  <si>
-    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>1 Anuidade - cartão básico nacional
-2 Anuidade - cartão básico internacional
-3 Fornecimento de 2ª via de cartão com função crédito
-4 Utilização de canais de atendimento para retirada em espécie no país
-5 Utilização de canais de atendimento para retirada em espécie no exterior
-6 Pagamento de contas utilizando a função crédito
-7 Avaliação emergencial de crédito</t>
-  </si>
-  <si>
-    <t>1 ANUIDADENacional
-2 ANUIDADEInt .
-3 2ª via-CARTÃOCRÉDITO
-4 RETIRADA-País
-5 RETIRADA-exterior
-6 PAGAMENTOCONTAS
-7 AVAL.EMERG.CRÉDITO</t>
-  </si>
-  <si>
-    <t>ANUIDADENacional
-"Disponibilização de rede de estabelecimentos afiliados, instalada no País, para pagamentos de bens e serviços, cobrada no máximo uma vez a cada doze meses, admitido o parcelamento da cobrança."
-ANUIDADEInt .
-"Disponibilização de rede de estabelecimentos afiliados, instalada no País e no exterior, para pagamentos de bens e serviços, cobrada no máximo uma vez a cada doze meses, admitido o parcelamento da cobrança."
-2ª via-CARTÃOCRÉDITO
-"Confecção e emissão de novo cartão com função crédito, restrito a casos de pedidos de reposição formulados pelo detentor do cartão, decorrente de perda, roubo, furto, danificação e outros motivos não imputáveis à instituição emitente."
-RETIRADA-País
-"Disponibilização e utilização pelo cliente de canais de atendimento disponíveis no País para retirada em espécie na função crédito."
-RETIRADA-exterior
-"Disponibilização e utilização pelo cliente de canais de atendimento disponíveis no exterior para retirada em espécie na função crédito ou débito."
-PAGAMENTOCONTAS
-"Realização de procedimentos operacionais para o pagamento de contas (água, luz, telefone, gás, tributos, boletos de cobrança, etc.), utilizando a função crédito do cartão"
-AVAL.EMERG.CRÉDITO
-"Avaliação de viabilidade e de riscos para a concessão de crédito em caráter emergencial, a pedido do cliente, por meio de atendimento pessoal, para realização de despesa acima do limite do cartão, cobrada no máximo uma vez nos últimos trinta dias."</t>
   </si>
   <si>
     <t>Denominação/Identificação do nome da conta.
 P.ex. "Cartão Universtiário Bem-Vindo"</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>productType</t>
   </si>
   <si>
     <r>
@@ -263,25 +140,39 @@
     </r>
   </si>
   <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>1 Classic Nacional
+2 Classic Internacional
+3 Gold
+4 Platinum
+5 Infinite
+6 Electron
+7 Standard Nacional
+8 Standard Internacional</t>
+  </si>
+  <si>
+    <t>brandCode</t>
+  </si>
+  <si>
     <t>Categoria de Bandeiras de Cartões.
 Bandeira é a detentora de todos os direitos e deveres da utilização da marca estampada no cartão, inclusive as bandeiras pertencentes aos emissores. p.ex. "American Express", "Diners Club".
 Essas bandeiras estão definidas em documento do BACEN de nome "Elaboração e Remessa de Informações Relativas aos Cartões de Pagamento  Emissores".</t>
   </si>
   <si>
-    <t>0 Não
-1 Sim</t>
-  </si>
-  <si>
-    <t>Indicador de arranjo de pagamento.
-Um arranjo de pagamento é o conjunto de regras e procedimentos que disciplina a prestação de determinado serviço de pagamento ao público.(Lei 12.865/2013, art. 6º, I).
-Podem ser 'Abertos' - quando o cartão de crédito não é associado a nenhuma marca/empresa em específico; ou 
-'Fechados' (Sim) - Os cartões de crédito private label são uma solução financeira que surgiu no Brasil em substituição aos sistemas de crediário para o consumidor. As cadeias de lojas passam a oferecer aos seus clientes um cartão de crédito com o seu nome, mas emitido por uma instituição financeira. Esses cartões private label são usados para oferecer crédito nas rede varejista, e voltados a um público de renda mais baixa.</t>
+    <t>1 VISA 
+2 MasterCard 
+3 American Express 
+4 Diners Club 
+5 Hipercard 
+6 Bandeira própria 
+7 Cheque Eletrônico 
+8 Elo 
+99 Outras</t>
   </si>
   <si>
     <t>hasProgramReward</t>
-  </si>
-  <si>
-    <t>programRewardInfo</t>
   </si>
   <si>
     <t>Indicador da existência de programa de fidelidade/recompensa associado à conta.
@@ -289,85 +180,200 @@
 1 Sim</t>
   </si>
   <si>
+    <t>Booleano</t>
+  </si>
+  <si>
+    <t>^([0-1]{1})$</t>
+  </si>
+  <si>
+    <t>0 Não
+1 Sim</t>
+  </si>
+  <si>
+    <t>programRewardInfo</t>
+  </si>
+  <si>
+    <t>Informações de Termos e condições do programa de fidelidade/recompensa. Pode ser informada a URL referente ao endereço onde constam as condições informadas.</t>
+  </si>
+  <si>
+    <t>Opcional</t>
+  </si>
+  <si>
     <t>Caso o campo "hasProgramReward"  indique que há programa de recompensa (1 - Sim), a informação de termos e condições deve ser preenchida.</t>
-  </si>
-  <si>
-    <t>Informações de Termos e condições do programa de fidelidade/recompensa. Pode ser informada a URL referente ao endereço onde constam as condições informadas.</t>
   </si>
   <si>
     <t>Nomes das Tarifas cobradas sobre Serviços relacionados à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa física. p.ex. "4 Utilização de canais de atendimento para retirada em espécie no país".
 Estes serviços são previstos na resolução 3.919 do BACEN.</t>
   </si>
   <si>
+    <t>1 Anuidade - cartão básico nacional
+2 Anuidade - cartão básico internacional
+3 Fornecimento de 2ª via de cartão com função crédito
+4 Utilização de canais de atendimento para retirada em espécie no país
+5 Utilização de canais de atendimento para retirada em espécie no exterior
+6 Pagamento de contas utilizando a função crédito
+7 Avaliação emergencial de crédito</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
     <t>Sigla de identificação do serviço relacionado à Modalidade de Contas de Pagamento Pós-Pagas para pessoa física informada. P.ex. "1 ANUIDADENacional". 
 Estas siglas são previstas na resolução 3.919 do BACEN.</t>
   </si>
   <si>
+    <t>1 ANUIDADENacional
+2 ANUIDADEInt .
+3 2ª via-CARTÃOCRÉDITO
+4 RETIRADA-País
+5 RETIRADA-exterior
+6 PAGAMENTOCONTAS
+7 AVAL.EMERG.CRÉDITO</t>
+  </si>
+  <si>
+    <t>chargeTriggerInfo</t>
+  </si>
+  <si>
     <t>Fatores geradores de cobrança que incidem sobre as Modalidades inforrmadas de Contas de Pagamento Pós-Pagas para pessoa física.Descrição sobre o Fato Estes fatos geradores são previstos na resolução 3.919 do BACEN.</t>
   </si>
   <si>
-    <t>chargeTriggerInfo</t>
+    <t>ANUIDADENacional
+"Disponibilização de rede de estabelecimentos afiliados, instalada no País, para pagamentos de bens e serviços, cobrada no máximo uma vez a cada doze meses, admitido o parcelamento da cobrança."
+ANUIDADEInt .
+"Disponibilização de rede de estabelecimentos afiliados, instalada no País e no exterior, para pagamentos de bens e serviços, cobrada no máximo uma vez a cada doze meses, admitido o parcelamento da cobrança."
+2ª via-CARTÃOCRÉDITO
+"Confecção e emissão de novo cartão com função crédito, restrito a casos de pedidos de reposição formulados pelo detentor do cartão, decorrente de perda, roubo, furto, danificação e outros motivos não imputáveis à instituição emitente."
+RETIRADA-País
+"Disponibilização e utilização pelo cliente de canais de atendimento disponíveis no País para retirada em espécie na função crédito."
+RETIRADA-exterior
+"Disponibilização e utilização pelo cliente de canais de atendimento disponíveis no exterior para retirada em espécie na função crédito ou débito."
+PAGAMENTOCONTAS
+"Realização de procedimentos operacionais para o pagamento de contas (água, luz, telefone, gás, tributos, boletos de cobrança, etc.), utilizando a função crédito do cartão"
+AVAL.EMERG.CRÉDITO
+"Avaliação de viabilidade e de riscos para a concessão de crédito em caráter emergencial, a pedido do cliente, por meio de atendimento pessoal, para realização de despesa acima do limite do cartão, cobrada no máximo uma vez nos últimos trinta dias."</t>
+  </si>
+  <si>
+    <t>maxPrice</t>
   </si>
   <si>
     <t>Valor máximo para a tarifa cobrada, relativa ao serviço relacionado à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa física. p.ex. 45,00</t>
   </si>
   <si>
+    <t>(\d{1,9}\,\d{2}){1}</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moeda referente ao valor da Tarifa, segundo modelo ISO-4217. p. ex. 'BRL' </t>
   </si>
   <si>
+    <t>^([A-Z]{3})$</t>
+  </si>
+  <si>
+    <t>Nomes das Tarifas cobradas sobre Serviços relacionados à Modalidade de Contas de Pagamento Pós-Pagas para pessoa física e que não estejam na resolução 3.919 do BACEN. p.ex. "Utilização de canais de atendimento via app".
+Caso não haja outro serviço, que não os prioritários, a estrutura de dados de outros serviços pode vir vazia, mas deve retornar ao menos uma.</t>
+  </si>
+  <si>
+    <t>Sigla de identificação do serviço relacionado à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa física e que não esteja, assim como o serviço, relacionada na resolução 3.919 do BACEN. p.ex. "ANUIDADADEUsoapp".
+Caso não haja outro serviço, que não os prioritários, a estrutura de dados de outros serviços pode vir vazia, mas deve retornar ao menos uma.</t>
+  </si>
+  <si>
+    <t>Fatores geradores de cobrança que incidem sobre as Modalidades de Contas de Pagamento Pós-Pagas para pessoa física e que não estejam relacionados a serviços previstos na resolução 3.919 do BACEN.
+Caso não haja outro serviço, que não os prioritários, a estrutura de dados de outros serviços pode vir vazia, mas deve retornar ao menos uma.</t>
+  </si>
+  <si>
+    <t>Valor máximo para a tarifa cobrada, relativa ao serviço relacionado à Modalidade de Contas de Pagamento Pós-Pagas para pessoa física e que não estejam previstos na resolução 3.919 do BACEN. p.ex. '45,00'.
+Caso não haja outro serviço, que não os prioritários, a estrutura de dados de outros serviços pode vir vazia, mas deve retornar ao menos uma.</t>
+  </si>
+  <si>
+    <t>Moeda referente ao valor da Tarifa, segundo modelo ISO-4217. p. ex. 'BRL' 
+Caso não haja outro serviço, que não os prioritários, a estrutura de dados de outros serviços pode vir vazia, mas deve retornar ao menos uma.</t>
+  </si>
+  <si>
+    <t>feeRate</t>
+  </si>
+  <si>
     <t>Percentual que corresponde a taxa aplicada para utilização de Crédito Rotativo. P.ex. '9,87%'</t>
   </si>
   <si>
+    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1} - pode ser N/A</t>
+  </si>
+  <si>
+    <t>instalmentRate</t>
+  </si>
+  <si>
     <t>Percentual que corresponde a taxa aplicada para pagamento parcelado do saldo devedor quando não realizado pagamento integral da fatura. P. Ex. '4,10%'.</t>
   </si>
   <si>
-    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1} - pode ser N/A</t>
-  </si>
-  <si>
     <t>Lista de outras operações de crédito. P.ex. '1 saque a crédito'</t>
   </si>
   <si>
+    <t>1 saque a crédito
+2 outros</t>
+  </si>
+  <si>
+    <t>minimumFeeRate</t>
+  </si>
+  <si>
     <t>Percentual para pagamento mínimo sobre o saldo devedor da fatura. P.ex. '25,00%'</t>
   </si>
   <si>
+    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
+  </si>
+  <si>
     <t>additionalInfo</t>
   </si>
   <si>
+    <t>Campo aberto para detalhamento de taxas de juros.</t>
+  </si>
+  <si>
+    <t>elegibilityCriteriaInfo</t>
+  </si>
+  <si>
     <t>Informação sobre as condições e critérios de elegibilidade do emissor do cartão. Pode ser informada a URL referente ao endereço onde constam as condições informadas.</t>
   </si>
   <si>
+    <t>closingProcessInfo</t>
+  </si>
+  <si>
     <t>Descrição dos procedimentos para encerramento da conta pós paga. Pode ser informada a URL referente ao endereço onde constam as condições informadas.</t>
   </si>
   <si>
-    <t>Nome da Instituição, pertencente à organização, responsável pelas contas de pagamento pós-pagas (cartões de crédito) Ex. 'Empresa da Organização A'</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>serviceName</t>
+    <t>Nomes das Tarifas cobradas sobre Serviços relacionados à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa jurídica. p.ex. "Utilização de canais de atendimento para retirada em espécie no país".
+Para as pessoas jurídicas, não há uma regulamentação específica sobre os serviços a serem prestados, como há para pessoas físicas.</t>
+  </si>
+  <si>
+    <t>Sigla de identificação do serviço relacionado à Modalidade de Contas de Pagamento Pós-Pagas para pessoa jurídica informada. P.ex. "ANUIDADENacional". 
+Para as pessoas jurídicas, não há uma regulamentação específica sobre os serviços a serem prestados, como há para pessoas físicas.</t>
   </si>
   <si>
     <t>Fatores geradores de cobrança que incidem sobre as Modalidades inforrmadas de Contas de Pagamento Pós-Pagas para pessoa jurídica.
 Para as pessoas jurídicas, não há uma regulamentação específica sobre os serviços a serem prestados, como há para pessoas físicas.</t>
   </si>
   <si>
-    <t>Sigla de identificação do serviço relacionado à Modalidade de Contas de Pagamento Pós-Pagas para pessoa jurídica informada. P.ex. "ANUIDADENacional". 
-Para as pessoas jurídicas, não há uma regulamentação específica sobre os serviços a serem prestados, como há para pessoas físicas.</t>
-  </si>
-  <si>
-    <t>Nomes das Tarifas cobradas sobre Serviços relacionados à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa jurídica. p.ex. "Utilização de canais de atendimento para retirada em espécie no país".
-Para as pessoas jurídicas, não há uma regulamentação específica sobre os serviços a serem prestados, como há para pessoas físicas.</t>
-  </si>
-  <si>
     <t>Valor máximo para a tarifa cobrada, relativa ao serviço relacionado à Modalidade informada de Contas de Pagamento Pós-Pagas para pessoa jurídica. p.ex. 45,00</t>
+  </si>
+  <si>
+    <t>Naturezas válidas: 
+Código, 
+Data, 
+Descrição, 
+Hora, 
+Indicador (Flag), 
+Nome, 
+Número, 
+Percentual, 
+Quantidade, 
+Texto, 
+Valor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,17 +836,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66" style="15" customWidth="1"/>
+    <col min="1" max="1" width="108.85546875" style="15" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="15" bestFit="1" customWidth="1"/>
@@ -854,64 +860,64 @@
     <col min="12" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/name</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="27">
         <v>30</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="18">
@@ -921,32 +927,32 @@
         <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="21" customFormat="1" ht="30">
       <c r="A3" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="27">
         <v>30</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="19">
@@ -956,35 +962,35 @@
         <v>1</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L3" s="20"/>
     </row>
-    <row r="4" spans="1:12" s="21" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="21" customFormat="1" ht="153.75" customHeight="1">
       <c r="A4" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="27">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I4" s="19">
         <v>1</v>
@@ -993,44 +999,44 @@
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/",B5)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/name</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="22">
         <v>50</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="18">
         <v>1</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="120">
       <c r="A6" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/",B6)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/productType</v>
@@ -1039,188 +1045,186 @@
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="22">
         <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I6" s="18">
         <v>1</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="135">
       <c r="A7" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/",B7)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/brandCode</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E7" s="22">
         <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I7" s="18">
         <v>1</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="60">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/",B8)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/identification/isPrivateLabel</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/",B8)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/hasProgramReward</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E8" s="22">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="I8" s="18">
         <v>1</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="60">
       <c r="A9" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/",B9)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/hasProgramReward</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/programRewardInfo</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" s="22">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="135">
+      <c r="A10" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/",B10)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/name</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="18">
-        <v>1</v>
-      </c>
-      <c r="J9" s="18" t="s">
+      <c r="C10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="22">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="23">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <v>7</v>
+      </c>
+      <c r="K10" s="24"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="105">
+      <c r="A11" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/",B11)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/code</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="22">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="33" t="s">
         <v>44</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/",B10)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/rewardsProgram/programRewardInfo</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="22">
-        <v>2000</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/",B11)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServiceName</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="22">
-        <v>50</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="I11" s="23">
         <v>1</v>
@@ -1231,29 +1235,29 @@
       <c r="K11" s="24"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="114" customHeight="1">
       <c r="A12" s="4" t="str">
-        <f t="shared" ref="A12:A15" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/code</v>
+        <f t="shared" ref="A12:A14" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/",B12)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/chargeTriggerInfo</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E12" s="22">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="33" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="I12" s="23">
         <v>1</v>
@@ -1261,64 +1265,64 @@
       <c r="J12" s="23">
         <v>7</v>
       </c>
-      <c r="K12" s="24"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="45">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/chargeTriggerInfo</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/maxPrice</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E13" s="22">
-        <v>300</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="23">
-        <v>1</v>
-      </c>
-      <c r="J13" s="23">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18">
         <v>7</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/maxPrice</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/priorityServices/currency</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E14" s="22">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="18">
@@ -1330,195 +1334,191 @@
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="90">
       <c r="A15" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/currency</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/",B15)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/name</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E15" s="22">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="18">
-        <v>1</v>
-      </c>
-      <c r="J15" s="18">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="23">
+        <v>1</v>
+      </c>
+      <c r="J15" s="23">
         <v>7</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="90">
       <c r="A16" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/",B16)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/feeRate</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>64</v>
+        <f t="shared" ref="A16:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/",B16)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/code</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E16" s="22">
+        <v>30</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="23">
+        <v>1</v>
+      </c>
+      <c r="J16" s="23">
         <v>7</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="18">
-        <v>1</v>
-      </c>
-      <c r="J16" s="18">
-        <v>1</v>
-      </c>
-      <c r="K16" s="7"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="114" customHeight="1">
       <c r="A17" s="4" t="str">
-        <f t="shared" ref="A17:A20" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/",B17)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/instalmentRate</v>
+        <f t="shared" si="1"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/chargeTriggerInfo</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="25">
+        <v>13</v>
+      </c>
+      <c r="E17" s="22">
+        <v>300</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="23">
+        <v>1</v>
+      </c>
+      <c r="J17" s="23">
         <v>7</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="18">
-        <v>1</v>
-      </c>
-      <c r="J17" s="18">
-        <v>1</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/code</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/maxPrice</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E18" s="22">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="26" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="18">
         <v>1</v>
       </c>
       <c r="J18" s="18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="str">
-        <f t="shared" ref="A19:A22" si="2">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/",B19)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/minimumFeeRate</v>
+    <row r="19" spans="1:12" ht="45">
+      <c r="A19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/fees/otherServices/currency</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E19" s="22">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="18">
         <v>1</v>
       </c>
       <c r="J19" s="18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/additionalInfo</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>37</v>
+    <row r="20" spans="1:12" ht="30">
+      <c r="A20" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/",B20)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/feeRate</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E20" s="22">
-        <v>500</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="H20" s="6"/>
       <c r="I20" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="18">
         <v>1</v>
@@ -1526,178 +1526,308 @@
       <c r="K20" s="7"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="str">
+    <row r="21" spans="1:12" ht="45">
+      <c r="A21" s="4" t="str">
+        <f t="shared" ref="A21:A24" si="2">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/",B21)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/instalmentRate</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="25">
+        <v>7</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="18">
+        <v>1</v>
+      </c>
+      <c r="J21" s="18">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" ht="30">
+      <c r="A22" s="4" t="str">
         <f t="shared" si="2"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/interestRates/code</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="22">
+        <v>30</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="18">
+        <v>1</v>
+      </c>
+      <c r="J22" s="18">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" ht="30">
+      <c r="A23" s="6" t="str">
+        <f t="shared" ref="A23:A26" si="3">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/",B23)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/minimumFeeRate</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="22">
+        <v>7</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="18">
+        <v>1</v>
+      </c>
+      <c r="J23" s="18">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/additionalInfo</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="22">
+        <v>500</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="18">
+        <v>0</v>
+      </c>
+      <c r="J24" s="18">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" s="21" customFormat="1" ht="45">
+      <c r="A25" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/elegibilityCriteriaInfo</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="27">
+      <c r="B25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="27">
         <v>2000</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="19">
-        <v>1</v>
-      </c>
-      <c r="J21" s="19">
-        <v>1</v>
-      </c>
-      <c r="K21" s="28"/>
-      <c r="L21" s="20"/>
-    </row>
-    <row r="22" spans="1:12" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="str">
-        <f t="shared" si="2"/>
+      <c r="F25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="19">
+        <v>1</v>
+      </c>
+      <c r="J25" s="19">
+        <v>1</v>
+      </c>
+      <c r="K25" s="28"/>
+      <c r="L25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" s="21" customFormat="1" ht="45">
+      <c r="A26" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalCreditCards/termsConditions/closingProcessInfo</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="27">
+      <c r="B26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="27">
         <v>2000</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="19">
-        <v>1</v>
-      </c>
-      <c r="J22" s="19">
-        <v>1</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="20"/>
-    </row>
-    <row r="24" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="19">
+        <v>1</v>
+      </c>
+      <c r="J26" s="19">
+        <v>1</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="20"/>
+    </row>
+    <row r="27" spans="1:12" s="21" customFormat="1">
+      <c r="A27" s="29"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="20"/>
+    </row>
+    <row r="28" spans="1:12" s="21" customFormat="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="20"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="7"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="31"/>
       <c r="H30" s="6"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="7"/>
       <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1706,17 +1836,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66" style="15" customWidth="1"/>
+    <col min="1" max="1" width="103.140625" style="15" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="15" bestFit="1" customWidth="1"/>
@@ -1730,64 +1860,64 @@
     <col min="12" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/name</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="27">
         <v>30</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="18">
@@ -1797,32 +1927,32 @@
         <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="21" customFormat="1" ht="30">
       <c r="A3" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="27">
         <v>30</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="19">
@@ -1832,35 +1962,35 @@
         <v>1</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L3" s="20"/>
     </row>
-    <row r="4" spans="1:12" s="21" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="21" customFormat="1" ht="153.75" customHeight="1">
       <c r="A4" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="27">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I4" s="19">
         <v>1</v>
@@ -1869,44 +1999,44 @@
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/",B5)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/name</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="22">
         <v>50</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="18">
         <v>1</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="120">
       <c r="A6" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/",B6)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/productType</v>
@@ -1915,187 +2045,183 @@
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="22">
         <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I6" s="18">
         <v>1</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="135">
       <c r="A7" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/",B7)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/brandCode</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E7" s="22">
         <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I7" s="18">
         <v>1</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="60">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/",B8)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/identification/isPrivateLabel</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/",B8)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/hasProgramReward</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E8" s="22">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="I8" s="18">
         <v>1</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="60">
       <c r="A9" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/",B9)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/hasProgramReward</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/programRewardInfo</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" s="22">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="75">
+      <c r="A10" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/",B10)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/name</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="18">
-        <v>1</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/",B10)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/rewardsProgram/programRewardInfo</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>57</v>
+      <c r="C10" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E10" s="22">
-        <v>2000</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>56</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="23">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <v>7</v>
+      </c>
+      <c r="K10" s="24"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="75">
       <c r="A11" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/",B11)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/serviceName</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/",B11)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/code</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E11" s="22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="23">
         <v>1</v>
       </c>
@@ -2105,90 +2231,92 @@
       <c r="K11" s="24"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="60">
       <c r="A12" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/code</v>
+        <f t="shared" ref="A12:A14" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/",B12)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/chargeTriggerInfo</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>76</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E12" s="22">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="33"/>
+        <v>14</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="23">
         <v>1</v>
       </c>
       <c r="J12" s="23">
         <v>7</v>
       </c>
-      <c r="K12" s="24"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="45">
       <c r="A13" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/chargeTriggerInfo</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/maxPrice</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>75</v>
+        <v>48</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E13" s="22">
-        <v>300</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="23">
-        <v>1</v>
-      </c>
-      <c r="J13" s="23">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18">
         <v>7</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/",B14)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/maxPrice</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/services/currency</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E14" s="22">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="18">
@@ -2200,61 +2328,61 @@
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/",B15)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/fees/currency</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>63</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/",B15)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/feeRate</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E15" s="22">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="18">
         <v>1</v>
       </c>
       <c r="J15" s="18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="45">
       <c r="A16" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/",B16)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/feeRate</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>64</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/instalmentRate</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="22">
+        <v>13</v>
+      </c>
+      <c r="E16" s="25">
         <v>7</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="18">
@@ -2266,30 +2394,30 @@
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/",B17)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/instalmentRate</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/code</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="22">
+        <v>30</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="25">
-        <v>7</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="6"/>
       <c r="I17" s="18">
         <v>1</v>
       </c>
@@ -2299,30 +2427,30 @@
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/",B18)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/interestRates/code</v>
+    <row r="18" spans="1:12" ht="30">
+      <c r="A18" s="6" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/",B18)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E18" s="22">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="26" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="18">
         <v>1</v>
       </c>
@@ -2332,32 +2460,30 @@
       <c r="K18" s="7"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="6" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/",B19)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E19" s="22">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>43</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="16"/>
       <c r="H19" s="6"/>
       <c r="I19" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="18">
         <v>1</v>
@@ -2365,141 +2491,124 @@
       <c r="K19" s="7"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="21" customFormat="1" ht="45">
       <c r="A20" s="6" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/",B20)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="22">
-        <v>500</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="27">
+        <v>2000</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="18">
-        <v>0</v>
-      </c>
-      <c r="J20" s="18">
-        <v>1</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H20" s="28"/>
+      <c r="I20" s="19">
+        <v>1</v>
+      </c>
+      <c r="J20" s="19">
+        <v>1</v>
+      </c>
+      <c r="K20" s="28"/>
+      <c r="L20" s="20"/>
+    </row>
+    <row r="21" spans="1:12" s="21" customFormat="1" ht="45">
       <c r="A21" s="6" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/",B21)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/closingProcessInfo</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E21" s="27">
         <v>2000</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="28"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="19">
         <v>1</v>
       </c>
       <c r="J21" s="19">
         <v>1</v>
       </c>
-      <c r="K21" s="28"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="1:12" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/",B22)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessCreditCards/termsConditions/closingProcessInfo</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="27">
-        <v>2000</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="16"/>
+    <row r="22" spans="1:12" s="21" customFormat="1">
+      <c r="A22" s="29"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="19">
-        <v>1</v>
-      </c>
-      <c r="J22" s="19">
-        <v>1</v>
-      </c>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
       <c r="K22" s="8"/>
       <c r="L22" s="20"/>
     </row>
-    <row r="23" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+    <row r="23" spans="1:12" s="21" customFormat="1">
+      <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
       <c r="K23" s="8"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="11"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="H25" s="7"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -2513,35 +2622,35 @@
       <c r="K26" s="7"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="7"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="7"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2555,23 +2664,9 @@
       <c r="K29" s="7"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="4"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I13" r:id="rId1" display="https://www.bcb.gov.br/Ftp/download/Descri%E7%E3o%20dos%20Servi%E7os%20Priorit%E1rios.pdf"/>
+    <hyperlink ref="I12" r:id="rId1" display="https://www.bcb.gov.br/Ftp/download/Descri%E7%E3o%20dos%20Servi%E7os%20Priorit%E1rios.pdf" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2579,21 +2674,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="198" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="198">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluídos os valores absolutos na cobrança de taxas
Incluídos os valores absolutos na cobrança de taxas
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
+++ b/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D9E1A3-5217-40D5-8240-648EFFB2B653}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7394D34-1265-494B-A7C2-F7DC769646AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="112">
   <si>
     <t>Xpath</t>
   </si>
@@ -118,19 +120,7 @@
     <t>^([A-Z]{3})$</t>
   </si>
   <si>
-    <t>feeRate</t>
-  </si>
-  <si>
-    <t>Percentual que corresponde a taxa aplicada para utilização de Crédito Rotativo. P.ex. '9,87%'</t>
-  </si>
-  <si>
     <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1} - pode ser N/A</t>
-  </si>
-  <si>
-    <t>instalmentRate</t>
-  </si>
-  <si>
-    <t>Percentual que corresponde a taxa aplicada para pagamento parcelado do saldo devedor quando não realizado pagamento integral da fatura. P. Ex. '4,10%'.</t>
   </si>
   <si>
     <t>minimumFeeRate</t>
@@ -472,6 +462,39 @@
   </si>
   <si>
     <t>Números de 0 a 9.</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>Identifica o período referente ao percentual de taxa de remuneração efetivamente aplicada no intervalo informado: mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
+  </si>
+  <si>
+    <t>Percentual para pagamento mínimo sobre o saldo devedor da fatura. p.ex. '25,00%'</t>
+  </si>
+  <si>
+    <t>Percentual que corresponde a taxa aplicada para pagamento parcelado do saldo devedor quando não realizado pagamento integral da fatura, no período informado. p.ex. '4,10%'.
+(representação de uma porcentagem Ex: 0.15 (O valor ao lado representa 15%. O valor 1 representa 100%))</t>
+  </si>
+  <si>
+    <t>Percentual que corresponde a taxa aplicada para utilização de Crédito Rotativo, no intervalo informado. p.ex. '9,87%'
+(representação de uma porcentagem Ex: 0.15 (O valor ao lado representa 15%. O valor 1 representa 100%))</t>
+  </si>
+  <si>
+    <t>Valor de referência utilizado na apuração dos percentuais informados por quartil
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeda relativa ao valor de referência, segundo modelo ISO-4217. p. ex. 'BRL' </t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>referenceValue</t>
+  </si>
+  <si>
+    <t>referenceCurrency</t>
   </si>
 </sst>
 </file>
@@ -535,7 +558,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +568,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -612,109 +641,148 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,6 +792,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -998,22 +1071,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="107.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="52" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -1049,10 +1122,10 @@
       <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="8"/>
@@ -1065,13 +1138,13 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>90</v>
+      <c r="C2" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1081,16 +1154,16 @@
         <v>14</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="20">
-        <v>1</v>
-      </c>
-      <c r="J2" s="20">
+      <c r="I2" s="19">
+        <v>1</v>
+      </c>
+      <c r="J2" s="19">
         <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="23"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" s="9" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -1101,12 +1174,12 @@
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1116,10 +1189,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="24">
-        <v>1</v>
-      </c>
-      <c r="J3" s="24">
+      <c r="I3" s="23">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
         <v>1</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -1135,12 +1208,12 @@
         <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1150,12 +1223,12 @@
         <v>17</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="24">
-        <v>1</v>
-      </c>
-      <c r="J4" s="24">
+        <v>101</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1</v>
+      </c>
+      <c r="J4" s="23">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1171,7 +1244,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -1186,10 +1259,10 @@
         <v>14</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="20">
-        <v>1</v>
-      </c>
-      <c r="J5" s="20" t="s">
+      <c r="I5" s="19">
+        <v>1</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K5" s="4"/>
@@ -1203,27 +1276,27 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="35">
+        <v>69</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="34">
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="20">
-        <v>1</v>
-      </c>
-      <c r="J6" s="20">
+        <v>60</v>
+      </c>
+      <c r="I6" s="19">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1232,31 +1305,31 @@
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/identification/",B7)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/identification/creditCardNetwork</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="34">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="35">
-        <v>100</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="20">
-        <v>1</v>
-      </c>
-      <c r="J7" s="20">
+      <c r="I7" s="19">
+        <v>1</v>
+      </c>
+      <c r="J7" s="19">
         <v>1</v>
       </c>
       <c r="K7" s="4"/>
@@ -1266,16 +1339,16 @@
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/identification/",B8)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/identification/additionalInfo</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="35">
+      <c r="B8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="34">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1285,14 +1358,14 @@
         <v>14</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>0</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>1</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -1301,10 +1374,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/rewardsProgram/hasRewardProgram</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -1315,12 +1388,12 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="20">
-        <v>1</v>
-      </c>
-      <c r="J9" s="20">
+        <v>72</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
         <v>1</v>
       </c>
       <c r="K9" s="4"/>
@@ -1331,7 +1404,7 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/rewardsProgram/rewardProgramInfo</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>22</v>
@@ -1346,14 +1419,14 @@
         <v>23</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>0</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,9 +1438,9 @@
         <v>24</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="10">
@@ -1377,63 +1450,63 @@
         <v>13</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="25">
-        <v>1</v>
-      </c>
-      <c r="J11" s="25">
+      <c r="H11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="24">
+        <v>1</v>
+      </c>
+      <c r="J11" s="24">
         <v>7</v>
       </c>
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="str">
+      <c r="A12" s="31" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/",B12)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/types</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="38">
+      <c r="B12" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="37">
         <v>30</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" s="40">
+      <c r="F12" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="39">
         <v>5</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="39">
         <v>5</v>
       </c>
-      <c r="K12" s="28" t="s">
-        <v>96</v>
+      <c r="K12" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="str">
+      <c r="A13" s="31" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/",B13)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/value</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>97</v>
+      <c r="B13" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>93</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -1445,25 +1518,25 @@
         <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="40">
+      <c r="I13" s="39">
         <v>5</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="39">
         <v>5</v>
       </c>
-      <c r="K13" s="28" t="s">
-        <v>96</v>
+      <c r="K13" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="str">
+      <c r="A14" s="31" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/",B14)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/price/currency</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1482,14 +1555,14 @@
         <v>27</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="40">
+      <c r="I14" s="39">
         <v>5</v>
       </c>
-      <c r="J14" s="40">
+      <c r="J14" s="39">
         <v>5</v>
       </c>
-      <c r="K14" s="28" t="s">
-        <v>96</v>
+      <c r="K14" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1498,10 +1571,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/chargingUnit</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1515,15 +1588,15 @@
       <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="20">
-        <v>1</v>
-      </c>
-      <c r="J15" s="20">
+      <c r="H15" s="18"/>
+      <c r="I15" s="19">
+        <v>1</v>
+      </c>
+      <c r="J15" s="19">
         <v>7</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -1535,7 +1608,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -1548,10 +1621,10 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="25">
-        <v>1</v>
-      </c>
-      <c r="J16" s="25" t="s">
+      <c r="I16" s="24">
+        <v>1</v>
+      </c>
+      <c r="J16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K16" s="11"/>
@@ -1565,7 +1638,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
@@ -1577,11 +1650,11 @@
         <v>13</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="25">
-        <v>1</v>
-      </c>
-      <c r="J17" s="25" t="s">
+      <c r="H17" s="17"/>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
+      <c r="J17" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K17" s="11"/>
@@ -1592,10 +1665,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/chargingTriggerInfo</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
@@ -1607,10 +1680,10 @@
         <v>13</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="25">
-        <v>1</v>
-      </c>
-      <c r="J18" s="25" t="s">
+      <c r="I18" s="24">
+        <v>1</v>
+      </c>
+      <c r="J18" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="4"/>
@@ -1621,34 +1694,34 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/type</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="42">
+        <v>42</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="41">
         <v>30</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="41">
+      <c r="F19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="40">
         <v>5</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="40">
         <v>5</v>
       </c>
-      <c r="K19" s="28" t="s">
-        <v>96</v>
+      <c r="K19" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1657,10 +1730,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/value</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -1668,21 +1741,21 @@
       <c r="E20" s="10">
         <v>12</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="41">
+      <c r="I20" s="40">
         <v>5</v>
       </c>
-      <c r="J20" s="41">
+      <c r="J20" s="40">
         <v>5</v>
       </c>
-      <c r="K20" s="28" t="s">
-        <v>96</v>
+      <c r="K20" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1694,7 +1767,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -1702,23 +1775,23 @@
       <c r="E21" s="10">
         <v>3</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="41">
+        <v>47</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="40">
         <v>5</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J21" s="40">
         <v>5</v>
       </c>
-      <c r="K21" s="28" t="s">
-        <v>96</v>
+      <c r="K21" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,10 +1800,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/additionalInfo</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
@@ -1744,15 +1817,15 @@
       <c r="G22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20">
+      <c r="H22" s="18"/>
+      <c r="I22" s="19">
         <v>0</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1761,10 +1834,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/chargingUnit</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -1778,370 +1851,586 @@
       <c r="G23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="20">
-        <v>1</v>
-      </c>
-      <c r="J23" s="20" t="s">
+      <c r="H23" s="18"/>
+      <c r="I23" s="19">
+        <v>1</v>
+      </c>
+      <c r="J23" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K23" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B24)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/types</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1">
+        <v>30</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="19">
+        <v>5</v>
+      </c>
+      <c r="J24" s="19">
+        <v>5</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B25)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/rate</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="10">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="52"/>
+      <c r="I25" s="19">
+        <v>5</v>
+      </c>
+      <c r="J25" s="19">
+        <v>5</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B26)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceValue</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="56">
+        <v>12</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B24)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="H26" s="57"/>
+      <c r="I26" s="56">
+        <v>1</v>
+      </c>
+      <c r="J26" s="56">
+        <v>1</v>
+      </c>
+      <c r="K26" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B27)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceCurrency</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="58">
+        <v>3</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="56">
+        <v>1</v>
+      </c>
+      <c r="J27" s="56">
+        <v>1</v>
+      </c>
+      <c r="K27" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B28)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/types</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="19">
+        <v>5</v>
+      </c>
+      <c r="J28" s="19">
+        <v>5</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B29)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/rate</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="53">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="H29" s="3"/>
+      <c r="I29" s="19">
+        <v>5</v>
+      </c>
+      <c r="J29" s="19">
+        <v>5</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B30)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceValue</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="56">
+        <v>12</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="57"/>
+      <c r="I30" s="56">
+        <v>1</v>
+      </c>
+      <c r="J30" s="56">
+        <v>1</v>
+      </c>
+      <c r="K30" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B31)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceCurrency</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="58">
+        <v>3</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="56">
+        <v>1</v>
+      </c>
+      <c r="J31" s="56">
+        <v>1</v>
+      </c>
+      <c r="K31" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B32)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/code</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="34">
+        <v>30</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="33"/>
+      <c r="H32" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="19">
+        <v>1</v>
+      </c>
+      <c r="J32" s="19">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B33)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/additionalInfo</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="34">
+        <v>50</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="44"/>
+      <c r="I33" s="19">
+        <v>0</v>
+      </c>
+      <c r="J33" s="19">
+        <v>1</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B34)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/minimumFeeRate</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="10">
+      <c r="C34" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="10">
         <v>7</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="20">
-        <v>1</v>
-      </c>
-      <c r="J24" s="20">
-        <v>1</v>
-      </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B25)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="F34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="H34" s="3"/>
+      <c r="I34" s="19">
+        <v>1</v>
+      </c>
+      <c r="J34" s="19">
+        <v>1</v>
+      </c>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B35)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/additionalInfo</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="12">
-        <v>7</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="20">
-        <v>1</v>
-      </c>
-      <c r="J25" s="20">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B26)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/code</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="35">
-        <v>30</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="I26" s="20">
-        <v>1</v>
-      </c>
-      <c r="J26" s="20">
-        <v>1</v>
-      </c>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B27)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/additionalInfo</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="10">
+        <v>500</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="19">
+        <v>0</v>
+      </c>
+      <c r="J35" s="19">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B36)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/elegibilityCriteriaInfo</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="13">
+        <v>2000</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="23">
+        <v>1</v>
+      </c>
+      <c r="J36" s="23">
+        <v>1</v>
+      </c>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B37)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/closingProcessInfo</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="35">
-        <v>50</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="45"/>
-      <c r="I27" s="20">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
-        <v>1</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B28)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/minimumFeeRate</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="10">
-        <v>7</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="20">
-        <v>1</v>
-      </c>
-      <c r="J28" s="20">
-        <v>1</v>
-      </c>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B29)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/additionalInfo</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="10">
-        <v>500</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="20">
-        <v>0</v>
-      </c>
-      <c r="J29" s="20">
-        <v>1</v>
-      </c>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B30)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/elegibilityCriteriaInfo</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="14">
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="13">
         <v>2000</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="24">
-        <v>1</v>
-      </c>
-      <c r="J30" s="24">
-        <v>1</v>
-      </c>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B31)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/closingProcessInfo</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="14">
-        <v>2000</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="24">
-        <v>1</v>
-      </c>
-      <c r="J31" s="24">
-        <v>1</v>
-      </c>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="4"/>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="23">
+        <v>1</v>
+      </c>
+      <c r="J37" s="23">
+        <v>1</v>
+      </c>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,18 +2440,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="109.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2204,10 +2493,10 @@
       <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="8"/>
@@ -2220,13 +2509,13 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>86</v>
+      <c r="C2" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -2236,16 +2525,16 @@
         <v>14</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="20">
-        <v>1</v>
-      </c>
-      <c r="J2" s="20">
+      <c r="I2" s="19">
+        <v>1</v>
+      </c>
+      <c r="J2" s="19">
         <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="23"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -2255,13 +2544,13 @@
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>90</v>
+      <c r="C3" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2271,10 +2560,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="24">
-        <v>1</v>
-      </c>
-      <c r="J3" s="24">
+      <c r="I3" s="23">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
         <v>1</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -2290,12 +2579,12 @@
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -2305,12 +2594,12 @@
         <v>17</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="24">
-        <v>1</v>
-      </c>
-      <c r="J4" s="24">
+        <v>101</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1</v>
+      </c>
+      <c r="J4" s="23">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -2326,7 +2615,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -2341,10 +2630,10 @@
         <v>14</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="20">
-        <v>1</v>
-      </c>
-      <c r="J5" s="20" t="s">
+      <c r="I5" s="19">
+        <v>1</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K5" s="4"/>
@@ -2358,12 +2647,12 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="35">
+        <v>77</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="34">
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -2371,12 +2660,12 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="20">
-        <v>1</v>
-      </c>
-      <c r="J6" s="20">
+        <v>60</v>
+      </c>
+      <c r="I6" s="19">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2385,16 +2674,16 @@
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/identification/",B7)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/identification/creditCardNetwork</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="35">
+      <c r="B7" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="34">
         <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2402,31 +2691,31 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="20">
-        <v>1</v>
-      </c>
-      <c r="J7" s="20">
+        <v>61</v>
+      </c>
+      <c r="I7" s="19">
+        <v>1</v>
+      </c>
+      <c r="J7" s="19">
         <v>1</v>
       </c>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="str">
+      <c r="A8" s="44" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/identification/",B8)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/identification/additionalInfo</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="35">
+      <c r="B8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="34">
         <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -2436,14 +2725,14 @@
         <v>14</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>0</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>1</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2452,10 +2741,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/rewardsProgram/hasRewardProgram</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -2470,12 +2759,12 @@
         <v>21</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="20">
-        <v>1</v>
-      </c>
-      <c r="J9" s="20">
+        <v>72</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
         <v>1</v>
       </c>
       <c r="K9" s="4"/>
@@ -2486,7 +2775,7 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/rewardsProgram/rewardProgramInfo</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>22</v>
@@ -2504,14 +2793,14 @@
         <v>14</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>0</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2523,7 +2812,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
@@ -2536,10 +2825,10 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="25">
-        <v>1</v>
-      </c>
-      <c r="J11" s="25" t="s">
+      <c r="I11" s="24">
+        <v>1</v>
+      </c>
+      <c r="J11" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="11"/>
@@ -2553,7 +2842,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>12</v>
@@ -2565,11 +2854,11 @@
         <v>13</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="25">
-        <v>1</v>
-      </c>
-      <c r="J12" s="25" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="24">
+        <v>1</v>
+      </c>
+      <c r="J12" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K12" s="11"/>
@@ -2580,10 +2869,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/chargingTriggerInfo</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -2595,10 +2884,10 @@
         <v>13</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="25">
-        <v>1</v>
-      </c>
-      <c r="J13" s="25" t="s">
+      <c r="I13" s="24">
+        <v>1</v>
+      </c>
+      <c r="J13" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="4"/>
@@ -2609,34 +2898,34 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/price/type</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="42">
+        <v>42</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="41">
         <v>30</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="41">
+      <c r="F14" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="40">
         <v>5</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="40">
         <v>5</v>
       </c>
-      <c r="K14" s="28" t="s">
-        <v>96</v>
+      <c r="K14" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2645,10 +2934,10 @@
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/price/value</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>83</v>
+        <v>44</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>79</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -2660,17 +2949,17 @@
         <v>13</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="20">
+      <c r="I15" s="19">
         <v>5</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="19">
         <v>5</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2682,7 +2971,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -2694,19 +2983,19 @@
         <v>13</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="20">
+        <v>47</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="19">
         <v>5</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="19">
         <v>5</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2714,13 +3003,13 @@
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B17)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/additionalInfo</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="45" t="s">
+      <c r="B17" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="10">
@@ -2732,15 +3021,15 @@
       <c r="G17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20">
+      <c r="H17" s="18"/>
+      <c r="I17" s="19">
         <v>0</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2748,13 +3037,13 @@
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B18)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/chargingUnit</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="45" t="s">
+      <c r="B18" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="10">
@@ -2766,369 +3055,585 @@
       <c r="G18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20">
-        <v>1</v>
-      </c>
-      <c r="J18" s="20" t="s">
+      <c r="H18" s="18"/>
+      <c r="I18" s="19">
+        <v>1</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B19)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/types</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="31">
+        <v>30</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="40">
+        <v>5</v>
+      </c>
+      <c r="J19" s="40">
+        <v>5</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/rate</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="41">
+        <v>7</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="47"/>
+      <c r="I20" s="40">
+        <v>5</v>
+      </c>
+      <c r="J20" s="40">
+        <v>5</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/referenceValue</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="56">
+        <v>12</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B19)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate</v>
-      </c>
-      <c r="B19" s="34" t="s">
+      <c r="H21" s="57"/>
+      <c r="I21" s="56">
+        <v>1</v>
+      </c>
+      <c r="J21" s="56">
+        <v>1</v>
+      </c>
+      <c r="K21" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B22)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/referenceCurrency</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="58">
+        <v>3</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="56">
+        <v>1</v>
+      </c>
+      <c r="J22" s="56">
+        <v>1</v>
+      </c>
+      <c r="K22" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/types</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="31">
+        <v>30</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="40">
+        <v>5</v>
+      </c>
+      <c r="J23" s="40">
+        <v>5</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B24)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/rate</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="48">
+        <v>7</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="H24" s="28"/>
+      <c r="I24" s="40">
+        <v>5</v>
+      </c>
+      <c r="J24" s="40">
+        <v>5</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B25)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/referenceValue</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="56">
+        <v>12</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="57"/>
+      <c r="I25" s="56">
+        <v>1</v>
+      </c>
+      <c r="J25" s="56">
+        <v>1</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B26)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/referenceCurrency</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="58">
+        <v>3</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="56">
+        <v>1</v>
+      </c>
+      <c r="J26" s="56">
+        <v>1</v>
+      </c>
+      <c r="K26" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B27)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/code</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="10">
+        <v>30</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="19">
+        <v>1</v>
+      </c>
+      <c r="J27" s="19">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B28)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/additionalInfo</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="10">
+        <v>50</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="19">
+        <v>0</v>
+      </c>
+      <c r="J28" s="19">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B29)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
+      </c>
+      <c r="B29" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="C29" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="10">
         <v>7</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="20">
-        <v>1</v>
-      </c>
-      <c r="J19" s="20">
-        <v>1</v>
-      </c>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B20)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate</v>
-      </c>
-      <c r="B20" s="45" t="s">
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="H29" s="3"/>
+      <c r="I29" s="19">
+        <v>1</v>
+      </c>
+      <c r="J29" s="19">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B30)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="12">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="20">
-        <v>1</v>
-      </c>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B21)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/code</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="10">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="20">
-        <v>1</v>
-      </c>
-      <c r="J21" s="20">
-        <v>1</v>
-      </c>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B22)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/additionalInfo</v>
-      </c>
-      <c r="B22" s="45" t="s">
+      <c r="C30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10">
+        <v>500</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="19">
+        <v>0</v>
+      </c>
+      <c r="J30" s="19">
+        <v>1</v>
+      </c>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B31)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="13">
+        <v>2000</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="23">
+        <v>1</v>
+      </c>
+      <c r="J31" s="23">
+        <v>1</v>
+      </c>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B32)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/closingProcessInfo</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="10">
-        <v>50</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="20">
-        <v>0</v>
-      </c>
-      <c r="J22" s="20">
-        <v>1</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B23)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="10">
-        <v>7</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="20">
-        <v>1</v>
-      </c>
-      <c r="J23" s="20">
-        <v>1</v>
-      </c>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B24)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="10">
-        <v>500</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="20">
-        <v>0</v>
-      </c>
-      <c r="J24" s="20">
-        <v>1</v>
-      </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B25)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="14">
+      <c r="C32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="13">
         <v>2000</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="24">
-        <v>1</v>
-      </c>
-      <c r="J25" s="24">
-        <v>1</v>
-      </c>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B26)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/closingProcessInfo</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="14">
-        <v>2000</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="24">
-        <v>1</v>
-      </c>
-      <c r="J26" s="24">
-        <v>1</v>
-      </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="4"/>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="23">
+        <v>1</v>
+      </c>
+      <c r="J32" s="23">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adicionado os valores de referência também para tarifas, além das taxas.
Adicionado os valores de referência também para tarifas, além das taxas.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
+++ b/DicionarioDeDados-Contas-Cartão_Crédito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7394D34-1265-494B-A7C2-F7DC769646AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C33177-2296-449D-81DD-0E4AE674FCB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContaPgtoPagoPF" sheetId="4" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="112">
   <si>
     <t>Xpath</t>
   </si>
@@ -1071,11 +1069,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,120 +1563,131 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/",B15)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/referenceValue</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="56">
+        <v>12</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="57"/>
+      <c r="I15" s="56">
+        <v>1</v>
+      </c>
+      <c r="J15" s="56">
+        <v>1</v>
+      </c>
+      <c r="K15" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/",B16)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/referenceCurrency</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="58">
+        <v>3</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" s="56">
+        <v>1</v>
+      </c>
+      <c r="J16" s="56">
+        <v>1</v>
+      </c>
+      <c r="K16" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/",B17)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/priorityServices/chargingUnit</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="10">
         <v>50</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="F17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19">
-        <v>1</v>
-      </c>
-      <c r="J15" s="19">
+      <c r="H17" s="18"/>
+      <c r="I17" s="19">
+        <v>1</v>
+      </c>
+      <c r="J17" s="19">
         <v>7</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B16)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/name</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="10">
-        <v>50</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="24">
-        <v>1</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B17)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/code</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="10">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="24">
-        <v>1</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B18)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/chargingTriggerInfo</v>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/name</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="10">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="7"/>
       <c r="I18" s="24">
         <v>1</v>
@@ -1686,103 +1695,92 @@
       <c r="J18" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/",B19)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/type</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="41">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B19)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/code</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10">
         <v>30</v>
       </c>
-      <c r="F19" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="40">
-        <v>5</v>
-      </c>
-      <c r="J19" s="40">
-        <v>5</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="24">
+        <v>1</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/",B20)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/value</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/chargingTriggerInfo</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="10">
-        <v>12</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="40">
-        <v>5</v>
-      </c>
-      <c r="J20" s="40">
-        <v>5</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="24">
+        <v>1</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/",B21)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/currency</v>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/type</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="10">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="41">
+        <v>30</v>
       </c>
       <c r="F21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>48</v>
+      <c r="G21" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="I21" s="40">
         <v>5</v>
@@ -1794,218 +1792,218 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B22)</f>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/",B22)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/value</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="10">
+        <v>12</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="40">
+        <v>5</v>
+      </c>
+      <c r="J22" s="40">
+        <v>5</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/price/currency</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="10">
+        <v>3</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="40">
+        <v>5</v>
+      </c>
+      <c r="J23" s="40">
+        <v>5</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B24)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/referenceValue</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="56">
+        <v>12</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="57"/>
+      <c r="I24" s="56">
+        <v>1</v>
+      </c>
+      <c r="J24" s="56">
+        <v>1</v>
+      </c>
+      <c r="K24" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B25)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/referenceCurrency</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="58">
+        <v>3</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="56">
+        <v>1</v>
+      </c>
+      <c r="J25" s="56">
+        <v>1</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B26)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/additionalInfo</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="D26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="10">
         <v>80</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="19">
+      <c r="H26" s="18"/>
+      <c r="I26" s="19">
         <v>0</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J26" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B23)</f>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/",B27)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/fees/otherServices/chargingUnit</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="10">
+      <c r="D27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="10">
         <v>50</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="F27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="19">
-        <v>1</v>
-      </c>
-      <c r="J23" s="19" t="s">
+      <c r="H27" s="18"/>
+      <c r="I27" s="19">
+        <v>1</v>
+      </c>
+      <c r="J27" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B24)</f>
+    <row r="28" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B28)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/types</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="1">
-        <v>30</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="19">
-        <v>5</v>
-      </c>
-      <c r="J24" s="19">
-        <v>5</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B25)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/rate</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="10">
-        <v>7</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="19">
-        <v>5</v>
-      </c>
-      <c r="J25" s="19">
-        <v>5</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B26)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceValue</v>
-      </c>
-      <c r="B26" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="56">
-        <v>12</v>
-      </c>
-      <c r="F26" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="56">
-        <v>1</v>
-      </c>
-      <c r="J26" s="56">
-        <v>1</v>
-      </c>
-      <c r="K26" s="54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B27)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceCurrency</v>
-      </c>
-      <c r="B27" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="58">
-        <v>3</v>
-      </c>
-      <c r="F27" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="I27" s="56">
-        <v>1</v>
-      </c>
-      <c r="J27" s="56">
-        <v>1</v>
-      </c>
-      <c r="K27" s="54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B28)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/types</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>89</v>
@@ -2038,21 +2036,21 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B29)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/rate</v>
-      </c>
-      <c r="B29" s="31" t="s">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B29)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/rate</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>105</v>
+      <c r="C29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="53">
+      <c r="E29" s="10">
         <v>7</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -2061,7 +2059,7 @@
       <c r="G29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="52"/>
       <c r="I29" s="19">
         <v>5</v>
       </c>
@@ -2072,10 +2070,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B30)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceValue</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B30)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceValue</v>
       </c>
       <c r="B30" s="54" t="s">
         <v>110</v>
@@ -2108,8 +2106,8 @@
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B31)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceCurrency</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/",B31)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/feeRate/referenceCurrency</v>
       </c>
       <c r="B31" s="54" t="s">
         <v>111</v>
@@ -2142,279 +2140,367 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B32)</f>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B32)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/types</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1">
+        <v>30</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I32" s="19">
+        <v>5</v>
+      </c>
+      <c r="J32" s="19">
+        <v>5</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B33)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/rate</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="53">
+        <v>7</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="19">
+        <v>5</v>
+      </c>
+      <c r="J33" s="19">
+        <v>5</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B34)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceValue</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="56">
+        <v>12</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="57"/>
+      <c r="I34" s="56">
+        <v>1</v>
+      </c>
+      <c r="J34" s="56">
+        <v>1</v>
+      </c>
+      <c r="K34" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/",B35)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/instalmentRate/referenceCurrency</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="58">
+        <v>3</v>
+      </c>
+      <c r="F35" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I35" s="56">
+        <v>1</v>
+      </c>
+      <c r="J35" s="56">
+        <v>1</v>
+      </c>
+      <c r="K35" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B36)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/code</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="34">
+      <c r="D36" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="34">
         <v>30</v>
       </c>
-      <c r="F32" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="43" t="s">
+      <c r="F36" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="33"/>
+      <c r="H36" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="I32" s="19">
-        <v>1</v>
-      </c>
-      <c r="J32" s="19">
-        <v>1</v>
-      </c>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B33)</f>
+      <c r="I36" s="19">
+        <v>1</v>
+      </c>
+      <c r="J36" s="19">
+        <v>1</v>
+      </c>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/",B37)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/interestRates/additionalInfo</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="34">
+      <c r="D37" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="34">
         <v>50</v>
       </c>
-      <c r="F33" s="42" t="s">
+      <c r="F37" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="33" t="s">
+      <c r="G37" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="44"/>
-      <c r="I33" s="19">
+      <c r="H37" s="44"/>
+      <c r="I37" s="19">
         <v>0</v>
       </c>
-      <c r="J33" s="19">
-        <v>1</v>
-      </c>
-      <c r="K33" s="12" t="s">
+      <c r="J37" s="19">
+        <v>1</v>
+      </c>
+      <c r="K37" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B34)</f>
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B38)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/minimumFeeRate</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="10">
+      <c r="D38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="10">
         <v>7</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="F38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="19">
-        <v>1</v>
-      </c>
-      <c r="J34" s="19">
-        <v>1</v>
-      </c>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B35)</f>
+      <c r="H38" s="3"/>
+      <c r="I38" s="19">
+        <v>1</v>
+      </c>
+      <c r="J38" s="19">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B39)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/additionalInfo</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="10">
+      <c r="D39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="10">
         <v>500</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="19">
+      <c r="H39" s="3"/>
+      <c r="I39" s="19">
         <v>0</v>
       </c>
-      <c r="J35" s="19">
-        <v>1</v>
-      </c>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B36)</f>
+      <c r="J39" s="19">
+        <v>1</v>
+      </c>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B40)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/elegibilityCriteriaInfo</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="13">
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="13">
         <v>2000</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="23">
-        <v>1</v>
-      </c>
-      <c r="J36" s="23">
-        <v>1</v>
-      </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B37)</f>
+      <c r="F40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="23">
+        <v>1</v>
+      </c>
+      <c r="J40" s="23">
+        <v>1</v>
+      </c>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/",B41)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalCreditCards/termsConditions/closingProcessInfo</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="13">
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="13">
         <v>2000</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="23">
-        <v>1</v>
-      </c>
-      <c r="J37" s="23">
-        <v>1</v>
-      </c>
-      <c r="K37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="4"/>
+      <c r="F41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="23">
+        <v>1</v>
+      </c>
+      <c r="J41" s="23">
+        <v>1</v>
+      </c>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="4"/>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" s="4"/>
@@ -2422,15 +2508,67 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="16"/>
       <c r="H45" s="3"/>
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
       <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2440,13 +2578,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29:B29"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,600 +3136,644 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B17)</f>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="str">
+        <f t="shared" ref="A17:A18" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/price/",B17)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/price/referenceValue</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="56">
+        <v>12</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="57"/>
+      <c r="I17" s="56">
+        <v>1</v>
+      </c>
+      <c r="J17" s="56">
+        <v>1</v>
+      </c>
+      <c r="K17" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="54" t="str">
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/price/referenceCurrency</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="58">
+        <v>3</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="56">
+        <v>1</v>
+      </c>
+      <c r="J18" s="56">
+        <v>1</v>
+      </c>
+      <c r="K18" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B19)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/additionalInfo</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B19" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C19" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="D19" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10">
         <v>80</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19">
+      <c r="H19" s="18"/>
+      <c r="I19" s="19">
         <v>0</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B18)</f>
+    <row r="20" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/",B20)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/fees/services/chargingUnit</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B20" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C20" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="10">
+      <c r="D20" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="10">
         <v>50</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19">
-        <v>1</v>
-      </c>
-      <c r="J18" s="19" t="s">
+      <c r="H20" s="18"/>
+      <c r="I20" s="19">
+        <v>1</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B19)</f>
+    <row r="21" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B21)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/types</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B21" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C21" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="31">
+      <c r="D21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="31">
         <v>30</v>
       </c>
-      <c r="F19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="31" t="s">
+      <c r="F21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="H21" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I21" s="40">
         <v>5</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J21" s="40">
         <v>5</v>
       </c>
-      <c r="K19" s="27" t="s">
+      <c r="K21" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B20)</f>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B22)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/rate</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B22" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C22" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="41">
+      <c r="D22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="41">
         <v>7</v>
       </c>
-      <c r="F20" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="31" t="s">
+      <c r="F22" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="47"/>
-      <c r="I20" s="40">
+      <c r="H22" s="47"/>
+      <c r="I22" s="40">
         <v>5</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J22" s="40">
         <v>5</v>
       </c>
-      <c r="K20" s="27" t="s">
+      <c r="K22" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B21)</f>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B23)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/referenceValue</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B23" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C23" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="56">
-        <v>12</v>
-      </c>
-      <c r="F21" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="57" t="s">
+      <c r="D23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="56">
+        <v>12</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="56">
-        <v>1</v>
-      </c>
-      <c r="J21" s="56">
-        <v>1</v>
-      </c>
-      <c r="K21" s="54" t="s">
+      <c r="H23" s="57"/>
+      <c r="I23" s="56">
+        <v>1</v>
+      </c>
+      <c r="J23" s="56">
+        <v>1</v>
+      </c>
+      <c r="K23" s="54" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B22)</f>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/",B24)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/feeRate/referenceCurrency</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B24" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C24" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="58">
+      <c r="D24" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="58">
         <v>3</v>
       </c>
-      <c r="F22" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="57" t="s">
+      <c r="F24" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H24" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="I22" s="56">
-        <v>1</v>
-      </c>
-      <c r="J22" s="56">
-        <v>1</v>
-      </c>
-      <c r="K22" s="54" t="s">
+      <c r="I24" s="56">
+        <v>1</v>
+      </c>
+      <c r="J24" s="56">
+        <v>1</v>
+      </c>
+      <c r="K24" s="54" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B23)</f>
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B25)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/types</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B25" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C25" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="31">
+      <c r="D25" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="31">
         <v>30</v>
       </c>
-      <c r="F23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="31" t="s">
+      <c r="F25" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="47" t="s">
+      <c r="H25" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I25" s="40">
         <v>5</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J25" s="40">
         <v>5</v>
       </c>
-      <c r="K23" s="27" t="s">
+      <c r="K25" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B24)</f>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B26)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/rate</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B26" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C26" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="48">
+      <c r="D26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="48">
         <v>7</v>
       </c>
-      <c r="F24" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="31" t="s">
+      <c r="F26" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="40">
+      <c r="H26" s="28"/>
+      <c r="I26" s="40">
         <v>5</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J26" s="40">
         <v>5</v>
       </c>
-      <c r="K24" s="27" t="s">
+      <c r="K26" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B25)</f>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B27)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/referenceValue</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B27" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C27" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="56">
-        <v>12</v>
-      </c>
-      <c r="F25" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="57" t="s">
+      <c r="D27" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="56">
+        <v>12</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="57"/>
-      <c r="I25" s="56">
-        <v>1</v>
-      </c>
-      <c r="J25" s="56">
-        <v>1</v>
-      </c>
-      <c r="K25" s="54" t="s">
+      <c r="H27" s="57"/>
+      <c r="I27" s="56">
+        <v>1</v>
+      </c>
+      <c r="J27" s="56">
+        <v>1</v>
+      </c>
+      <c r="K27" s="54" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B26)</f>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/",B28)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/instalmentRate/referenceCurrency</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B28" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C28" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="58">
+      <c r="D28" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="58">
         <v>3</v>
       </c>
-      <c r="F26" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="57" t="s">
+      <c r="F28" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="59" t="s">
+      <c r="H28" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="I26" s="56">
-        <v>1</v>
-      </c>
-      <c r="J26" s="56">
-        <v>1</v>
-      </c>
-      <c r="K26" s="54" t="s">
+      <c r="I28" s="56">
+        <v>1</v>
+      </c>
+      <c r="J28" s="56">
+        <v>1</v>
+      </c>
+      <c r="K28" s="54" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B27)</f>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B29)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/code</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B29" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C29" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="10">
+      <c r="D29" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="10">
         <v>30</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="30" t="s">
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="19">
-        <v>1</v>
-      </c>
-      <c r="J27" s="19">
-        <v>1</v>
-      </c>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B28)</f>
+      <c r="I29" s="19">
+        <v>1</v>
+      </c>
+      <c r="J29" s="19">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/",B30)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/interestRates/additionalInfo</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B30" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C30" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="10">
+      <c r="D30" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10">
         <v>50</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="19">
-        <v>0</v>
-      </c>
-      <c r="J28" s="19">
-        <v>1</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B29)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="10">
-        <v>7</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="19">
-        <v>1</v>
-      </c>
-      <c r="J29" s="19">
-        <v>1</v>
-      </c>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B30)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="10">
-        <v>500</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="3"/>
       <c r="I30" s="19">
         <v>0</v>
       </c>
       <c r="J30" s="19">
         <v>1</v>
       </c>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="K30" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B31)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="13">
-        <v>2000</v>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/minimumFeeRate</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="10">
+        <v>7</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="23">
-        <v>1</v>
-      </c>
-      <c r="J31" s="23">
-        <v>1</v>
-      </c>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="19">
+        <v>1</v>
+      </c>
+      <c r="J31" s="19">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B32)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/additionalInfo</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="10">
+        <v>500</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="19">
+        <v>0</v>
+      </c>
+      <c r="J32" s="19">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B33)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/elegibilityCriteriaInfo</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="13">
+        <v>2000</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="23">
+        <v>1</v>
+      </c>
+      <c r="J33" s="23">
+        <v>1</v>
+      </c>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/",B34)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessCreditCards/termsConditions/closingProcessInfo</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="13">
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="13">
         <v>2000</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="23">
-        <v>1</v>
-      </c>
-      <c r="J32" s="23">
-        <v>1</v>
-      </c>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
+      <c r="F34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="23">
+        <v>1</v>
+      </c>
+      <c r="J34" s="23">
+        <v>1</v>
+      </c>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="4"/>
+    <row r="35" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="3"/>
+      <c r="H37" s="4"/>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" s="4"/>
@@ -3603,8 +3785,8 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="4"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="3"/>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="4"/>
@@ -3612,11 +3794,11 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="4"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="16"/>
       <c r="H39" s="3"/>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
@@ -3625,15 +3807,41 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>